<commit_message>
Nested row groupings: Fix several issues, generalize implementation to arbitrary nesting
-) groupRows did not properly overwrite existing groupings / append new ones
-) Add new parameter level = -1 to the groupRows funtion to let openxlsx auto-detect the next grouping level
-) Add test cast with several nested and unnested groupings to cover most use-cases
-) Saving to an .xlsx file dropped the grouping if a row didn't contain content any
-) Simplified xml-generation for grouped rows and row height.

Fixes part of #138, implements the counterpart of #105 for rows, and properly implements the remaining missing parts of #294.
</commit_message>
<xml_diff>
--- a/inst/extdata/nested_grouped_rowscols.xlsx
+++ b/inst/extdata/nested_grouped_rowscols.xlsx
@@ -5,25 +5,26 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R\openxlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R\openxlsx\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B96454-6D6B-4C7F-A820-FF90F3AA7C18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE35FFC7-4524-46A6-9013-EC7F7AC64771}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11835" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="simple visible grouping" sheetId="1" r:id="rId1"/>
     <sheet name="simple hidden grouping" sheetId="4" r:id="rId2"/>
-    <sheet name="nested grouping" sheetId="3" r:id="rId3"/>
-    <sheet name="nested grouping 2" sheetId="2" r:id="rId4"/>
+    <sheet name="multiple non-nested groupings" sheetId="5" r:id="rId3"/>
+    <sheet name="nested grouping" sheetId="2" r:id="rId4"/>
+    <sheet name="nested grouping 2" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Nested Grouping (rows and columns)</t>
   </si>
@@ -86,6 +87,27 @@
   </si>
   <si>
     <t>Simple Grouping (rows and columns; hidden)</t>
+  </si>
+  <si>
+    <t>Multiple groupings (non-overlapping rows and columns; visible)</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>F6</t>
   </si>
 </sst>
 </file>
@@ -505,7 +527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" defaultGridColor="0" colorId="22" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" defaultGridColor="0" colorId="22" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -560,44 +582,61 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5C4EAD-3222-47C7-93E6-DD2474E1609C}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C3BCC1B-EBC3-427B-8AB2-08EC27DF5176}">
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView showGridLines="0" defaultGridColor="0" colorId="22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView showGridLines="0" tabSelected="1" defaultGridColor="0" colorId="22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" outlineLevel="1"/>
-    <col min="2" max="3" width="11.5703125" outlineLevel="2"/>
-    <col min="4" max="4" width="11.5703125" outlineLevel="1"/>
+    <col min="1" max="2" width="11.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="5" width="11.5703125" outlineLevel="1"/>
+    <col min="7" max="8" width="0" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="11.5703125" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" outlineLevel="2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" outlineLevel="2" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="4" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:6" collapsed="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -613,14 +652,14 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showGridLines="0" defaultGridColor="0" colorId="22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="T26" sqref="T26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5703125" outlineLevel="1"/>
-    <col min="2" max="3" width="0" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="11.5703125" outlineLevel="1" collapsed="1"/>
+    <col min="2" max="3" width="11.5703125" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="11.5703125" outlineLevel="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -640,7 +679,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -654,7 +693,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -668,7 +707,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -700,4 +739,47 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5C4EAD-3222-47C7-93E6-DD2474E1609C}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView showGridLines="0" defaultGridColor="0" colorId="22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" outlineLevel="1"/>
+    <col min="2" max="3" width="11.5703125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="11.5703125" outlineLevel="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:2" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>